<commit_message>
pain final edits to format
</commit_message>
<xml_diff>
--- a/_data/pp_recs_all.xlsx
+++ b/_data/pp_recs_all.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mgrant/Documents/_projects/r/pp_recs/_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B78122B1-7D83-764C-B4E8-76785650C3B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DECB49AF-85CA-D64E-9528-ABB20C6AE0D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="500" windowWidth="43700" windowHeight="28160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1995,12 +1995,12 @@
     <t>subrec</t>
   </si>
   <si>
-    <t>Institutional Policies and Procedures for Providing Perioperative Pain Management</t>
-  </si>
-  <si>
-    <t>Anesthesiologists offering perioperative analgesia services should provide, in collaboration with other healthcare professionals as appropriate, ongoing education and training to ensure that hospital personnel are knowledgeable and skilled with regard to the effective and safe use of the available treatment options within the institution.&lt;br/&gt;&lt;br/&gt;
+    <t>Anesthesiologists offering perioperative analgesia services should provide, in collaboration with other healthcare professionals as appropriate, ongoing education and training to ensure that hospital personnel are knowledgeable and skilled with regard to the effective and safe use of the available treatment options within the institution.&lt;br/&gt;
 &amp;#9702; &lt;font size = 3&gt;  Educational content should range from basic bedside pain assessment to sophisticated pain management techniques (e.g., epidural analgesia, PCA, and various regional anesthesia techniques) and nonpharmacologic techniques (e.g., relaxation, imagery, hypnotic methods).&lt;br/&gt;
 &amp;#9702; For optimal pain management, ongoing education and training are essential for new personnel, to maintain skills, and whenever therapeutic approaches are modified.&lt;/font&gt;</t>
+  </si>
+  <si>
+    <t>Institutional Policies and Procedures for Providing Perioperative Pain Management</t>
   </si>
 </sst>
 </file>
@@ -8960,10 +8960,10 @@
         <v>2012</v>
       </c>
       <c r="D325" s="9" t="s">
+        <v>639</v>
+      </c>
+      <c r="E325" s="9" t="s">
         <v>638</v>
-      </c>
-      <c r="E325" s="9" t="s">
-        <v>639</v>
       </c>
       <c r="F325" s="11" t="s">
         <v>586</v>
@@ -8981,7 +8981,7 @@
         <v>2012</v>
       </c>
       <c r="D326" s="9" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="E326" s="9" t="s">
         <v>636</v>
@@ -9002,7 +9002,7 @@
         <v>2012</v>
       </c>
       <c r="D327" s="9" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="E327" s="9" t="s">
         <v>465</v>
@@ -9022,7 +9022,7 @@
         <v>2012</v>
       </c>
       <c r="D328" s="9" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="E328" s="9" t="s">
         <v>466</v>
@@ -9042,7 +9042,7 @@
         <v>2012</v>
       </c>
       <c r="D329" s="9" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="E329" s="9" t="s">
         <v>467</v>
@@ -9062,7 +9062,7 @@
         <v>2012</v>
       </c>
       <c r="D330" s="9" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="E330" s="9" t="s">
         <v>468</v>
@@ -9082,7 +9082,7 @@
         <v>2012</v>
       </c>
       <c r="D331" s="9" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="E331" s="9" t="s">
         <v>469</v>
@@ -9102,7 +9102,7 @@
         <v>2012</v>
       </c>
       <c r="D332" s="9" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="E332" s="9" t="s">
         <v>470</v>

</xml_diff>

<commit_message>
fix col label, hyphens
</commit_message>
<xml_diff>
--- a/_data/pp_recs_all.xlsx
+++ b/_data/pp_recs_all.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mgrant/Documents/_projects/r/pp_recs/_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A61939CD-1980-1B4F-8FC6-7C182DCE0DDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8226348E-72CB-B240-8316-0B9896D00638}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="500" windowWidth="43700" windowHeight="28160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2070,22 +2070,22 @@
     <t xml:space="preserve">We recommend against using eye muscles for neuromuscular monitoring.  </t>
   </si>
   <si>
-    <t>We suggest neostigmine as a reason-able alternative to sugammadex at mini-mal depth of neuromuscular blockade.</t>
-  </si>
-  <si>
     <t>To avoid residual neuromuscular blockade when atracurium or cisatracurium are administered and qualitative assessment is used, we suggest antagonism with neostigmine at minimal neuromuscular blockade depth. In the absence of quantitative monitoring, at least 10 min should elapse from antagonism to extubation. When quantitative monitoring is utilized, extubation can be done as soon as a train-of-four ratio greater than or equal to 0.9 is confirmed before extubation.</t>
   </si>
   <si>
     <t>Deep: posttetanic count greater than or equal to 1 and train-of-four count 0; mod-erate: train-of-four count 1 to 3; shallow: train-of-four count 4 and train-of-four ratio less than 0.4; minimal: train-of-four ratio 0.4 to less than 0.9.</t>
   </si>
   <si>
-    <t>We recommend sugammadex over neostigmine at deep, moderate, and shallow depths of neuromuscular blockade induced by rocuronium or vecuronium, to avoid residual neuro-muscular blockade.</t>
-  </si>
-  <si>
     <t>Low</t>
   </si>
   <si>
     <t>foot_note</t>
+  </si>
+  <si>
+    <t>We suggest neostigmine as a reasonable alternative to sugammadex at mini-mal depth of neuromuscular blockade.</t>
+  </si>
+  <si>
+    <t>We recommend sugammadex over neostigmine at deep, moderate, and shallow depths of neuromuscular blockade induced by rocuronium or vecuronium, to avoid residual neuromuscular blockade.</t>
   </si>
 </sst>
 </file>
@@ -12118,7 +12118,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -12148,7 +12148,7 @@
         <v>640</v>
       </c>
       <c r="F1" s="29" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="160" x14ac:dyDescent="0.2">
@@ -12335,7 +12335,7 @@
         <v>2023</v>
       </c>
       <c r="C12" s="29" t="s">
-        <v>665</v>
+        <v>667</v>
       </c>
       <c r="D12" s="28" t="s">
         <v>625</v>
@@ -12344,7 +12344,7 @@
         <v>647</v>
       </c>
       <c r="F12" s="29" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -12355,13 +12355,13 @@
         <v>2023</v>
       </c>
       <c r="C13" s="29" t="s">
-        <v>662</v>
+        <v>666</v>
       </c>
       <c r="D13" s="28" t="s">
         <v>651</v>
       </c>
       <c r="E13" s="28" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="96" x14ac:dyDescent="0.2">
@@ -12372,7 +12372,7 @@
         <v>2023</v>
       </c>
       <c r="C14" s="29" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="D14" s="28" t="s">
         <v>651</v>

</xml_diff>